<commit_message>
corrected chla dataframe to include volume-adjusted estimates, added treatment names to hobo data, and added treatment column to density data.
</commit_message>
<xml_diff>
--- a/data/biol_402_epiphyte_shoots.xlsx
+++ b/data/biol_402_epiphyte_shoots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryoconnor/Github/Biol402/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryo/GitHub/biol_402/Biol_402_2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26CD0E9-1FAF-8340-AA2D-2D51055FDDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C43BB80-D604-774D-B552-8AF1F600CD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="34980" windowHeight="17040" xr2:uid="{EBDD8445-C656-B04F-BA9A-67D36C56F22E}"/>
+    <workbookView xWindow="500" yWindow="2480" windowWidth="22980" windowHeight="12560" xr2:uid="{EBDD8445-C656-B04F-BA9A-67D36C56F22E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -544,10 +544,10 @@
   <dimension ref="A1:AC999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD21"/>
+      <selection pane="bottomRight" activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -702,9 +702,10 @@
         <v>136.65</v>
       </c>
       <c r="V2" s="10">
-        <v>310.56818179999999</v>
-      </c>
-      <c r="W2" s="1"/>
+        <f>((U2*(T2/R2)*5)*(100/P2))/1000</f>
+        <v>310.56818181818181</v>
+      </c>
+      <c r="W2" s="10"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
@@ -776,6 +777,7 @@
         <v>122.75</v>
       </c>
       <c r="V3" s="10">
+        <f t="shared" ref="V3:V25" si="1">((U3*(T3/R3)*5)*(100/P3))/1000</f>
         <v>245.5</v>
       </c>
       <c r="W3" s="1"/>
@@ -845,6 +847,7 @@
         <v>68.56</v>
       </c>
       <c r="V4" s="10">
+        <f t="shared" si="1"/>
         <v>137.12</v>
       </c>
       <c r="W4" s="1"/>
@@ -918,7 +921,8 @@
       <c r="U5" s="1">
         <v>61.295000000000002</v>
       </c>
-      <c r="V5" s="1">
+      <c r="V5" s="10">
+        <f t="shared" si="1"/>
         <v>61.295000000000002</v>
       </c>
       <c r="W5" s="1"/>
@@ -992,7 +996,8 @@
       <c r="U6" s="1">
         <v>102.1</v>
       </c>
-      <c r="V6" s="1">
+      <c r="V6" s="10">
+        <f t="shared" si="1"/>
         <v>204.2</v>
       </c>
       <c r="W6" s="1"/>
@@ -1066,7 +1071,8 @@
       <c r="U7" s="1">
         <v>123.65</v>
       </c>
-      <c r="V7" s="1">
+      <c r="V7" s="10">
+        <f t="shared" si="1"/>
         <v>494.6</v>
       </c>
       <c r="W7" s="1"/>
@@ -1135,7 +1141,8 @@
       <c r="U8" s="1">
         <v>60.71</v>
       </c>
-      <c r="V8" s="1">
+      <c r="V8" s="10">
+        <f t="shared" si="1"/>
         <v>12.141999999999999</v>
       </c>
       <c r="W8" s="1"/>
@@ -1204,7 +1211,8 @@
       <c r="U9" s="1">
         <v>88.58</v>
       </c>
-      <c r="V9" s="1">
+      <c r="V9" s="10">
+        <f t="shared" si="1"/>
         <v>88.58</v>
       </c>
       <c r="W9" s="1"/>
@@ -1278,7 +1286,8 @@
       <c r="U10" s="5">
         <v>90.03</v>
       </c>
-      <c r="V10" s="5">
+      <c r="V10" s="10">
+        <f t="shared" si="1"/>
         <v>180.06</v>
       </c>
       <c r="W10" s="5"/>
@@ -1345,7 +1354,8 @@
       <c r="U11" s="5">
         <v>166.9</v>
       </c>
-      <c r="V11" s="5">
+      <c r="V11" s="10">
+        <f t="shared" si="1"/>
         <v>333.8</v>
       </c>
       <c r="W11" s="5"/>
@@ -1405,8 +1415,9 @@
       <c r="U12" s="5">
         <v>235.1</v>
       </c>
-      <c r="V12" s="5">
-        <v>559.76190480000002</v>
+      <c r="V12" s="10">
+        <f t="shared" si="1"/>
+        <v>559.7619047619047</v>
       </c>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
@@ -1478,7 +1489,8 @@
       <c r="U13" s="1">
         <v>84.16</v>
       </c>
-      <c r="V13" s="1">
+      <c r="V13" s="10">
+        <f t="shared" si="1"/>
         <v>84.16</v>
       </c>
       <c r="W13" s="1"/>
@@ -1552,8 +1564,9 @@
       <c r="U14" s="1">
         <v>54.034999999999997</v>
       </c>
-      <c r="V14" s="1">
-        <v>108.07</v>
+      <c r="V14" s="10">
+        <f t="shared" si="1"/>
+        <v>108.06999999999998</v>
       </c>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
@@ -1623,7 +1636,8 @@
       <c r="U15" s="1">
         <v>110.6</v>
       </c>
-      <c r="V15" s="1">
+      <c r="V15" s="10">
+        <f t="shared" si="1"/>
         <v>110.6</v>
       </c>
       <c r="W15" s="1"/>
@@ -1697,7 +1711,8 @@
       <c r="U16" s="1">
         <v>83.89</v>
       </c>
-      <c r="V16" s="1">
+      <c r="V16" s="10">
+        <f t="shared" si="1"/>
         <v>83.89</v>
       </c>
       <c r="W16" s="1"/>
@@ -1771,7 +1786,8 @@
       <c r="U17" s="1">
         <v>115.35</v>
       </c>
-      <c r="V17" s="1">
+      <c r="V17" s="10">
+        <f t="shared" si="1"/>
         <v>23.07</v>
       </c>
       <c r="W17" s="1"/>
@@ -1847,8 +1863,9 @@
       <c r="U18" s="6">
         <v>243</v>
       </c>
-      <c r="V18" s="5">
-        <v>725.37313429999995</v>
+      <c r="V18" s="10">
+        <f t="shared" si="1"/>
+        <v>725.37313432835822</v>
       </c>
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
@@ -1921,7 +1938,8 @@
       <c r="U19" s="1">
         <v>72.849999999999994</v>
       </c>
-      <c r="V19" s="1">
+      <c r="V19" s="10">
+        <f t="shared" si="1"/>
         <v>72.849999999999994</v>
       </c>
       <c r="W19" s="1"/>
@@ -1986,7 +2004,8 @@
       <c r="U20" s="5">
         <v>166.9</v>
       </c>
-      <c r="V20" s="5">
+      <c r="V20" s="10">
+        <f t="shared" si="1"/>
         <v>333.8</v>
       </c>
       <c r="W20" s="5"/>
@@ -2037,7 +2056,7 @@
       <c r="U21" s="5">
         <v>53.42</v>
       </c>
-      <c r="V21" s="6"/>
+      <c r="V21" s="10"/>
       <c r="W21" s="5"/>
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
@@ -2106,8 +2125,9 @@
       <c r="U22" s="5">
         <v>101.59</v>
       </c>
-      <c r="V22" s="5">
-        <v>338.6333333</v>
+      <c r="V22" s="10">
+        <f t="shared" si="1"/>
+        <v>338.63333333333338</v>
       </c>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
@@ -2180,8 +2200,9 @@
       <c r="U23" s="1">
         <v>77.59</v>
       </c>
-      <c r="V23" s="1">
-        <v>258.6333333</v>
+      <c r="V23" s="10">
+        <f t="shared" si="1"/>
+        <v>258.63333333333338</v>
       </c>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
@@ -2252,6 +2273,7 @@
         <v>40.15</v>
       </c>
       <c r="V24" s="10">
+        <f t="shared" si="1"/>
         <v>40.15</v>
       </c>
       <c r="W24" s="5"/>
@@ -2321,7 +2343,7 @@
       <c r="U25" s="1">
         <v>262.8</v>
       </c>
-      <c r="V25" s="2"/>
+      <c r="V25" s="10"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>

</xml_diff>